<commit_message>
tested basic model functionality
</commit_message>
<xml_diff>
--- a/dairyclimatemodel/data/ghg_params.xlsx
+++ b/dairyclimatemodel/data/ghg_params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\household_ghg_model\household_ghg_model\dairyclimatemodel2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hawkj\Documents\GitHub\household_ghg_model\dairyclimatemodel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7649578E-5A2B-46F6-9BCE-D2B5AA639DEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEE1BC1-734E-4016-8239-E20ED540173B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="108" windowWidth="23256" windowHeight="12600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,14 @@
     <sheet name="CO2_Fossil_Fuel" sheetId="6" r:id="rId7"/>
     <sheet name="allocation_factor" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1166,15 +1173,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:F2"/>
+  <dimension ref="B1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -1184,11 +1191,11 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <f>0.0786*1000</f>
         <v>78.600000000000009</v>
@@ -1201,7 +1208,7 @@
         <f>0.0786*1000</f>
         <v>78.600000000000009</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>